<commit_message>
Update Automation Exercise Website API Test Cases.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Automation Exercise Website API Test Cases.xlsx
+++ b/Documents/Automation Exercise Website API Test Cases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="200">
   <si>
     <t>ID</t>
   </si>
@@ -53,12 +53,154 @@
     <t>TC_API08_001</t>
   </si>
   <si>
+    <t>Verify login without email parameter</t>
+  </si>
+  <si>
+    <t>/api/verifyLogin</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>{ "password": "Abc@1234" }</t>
+  </si>
+  <si>
+    <t>{"responseCode": 400, "message": "Bad request, email or password parameter is missing in POST request."}</t>
+  </si>
+  <si>
     <t>NotTested</t>
   </si>
   <si>
+    <t>Critical</t>
+  </si>
+  <si>
     <t>Muhammad EmadEl-dien Ali</t>
   </si>
   <si>
+    <t>TC_API08_002</t>
+  </si>
+  <si>
+    <t>Verify login without password parameter</t>
+  </si>
+  <si>
+    <t>{ "email": "test1233@example.com" }</t>
+  </si>
+  <si>
+    <t>TC_API08_003</t>
+  </si>
+  <si>
+    <t>Verify login without both email &amp; password</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>TC_API08_004</t>
+  </si>
+  <si>
+    <t>Verify login with empty email value</t>
+  </si>
+  <si>
+    <t>{ "email": "", "password": "Abc@1234" }</t>
+  </si>
+  <si>
+    <t>{"responseCode": 404, "message": "User not found!"}</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>TC_API08_005</t>
+  </si>
+  <si>
+    <t>Verify login with empty password value</t>
+  </si>
+  <si>
+    <t>{ "email": "test1233@example.com", "password": "" }</t>
+  </si>
+  <si>
+    <t>TC_API08_006</t>
+  </si>
+  <si>
+    <t>Verify login with non-existing or invalid email</t>
+  </si>
+  <si>
+    <t>{ "email": "notfound@example", "password": "12345" }</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>TC_API08_007</t>
+  </si>
+  <si>
+    <t>Verify login with correct email and wrong password</t>
+  </si>
+  <si>
+    <t>{ "email": "test1233@example.com", "password": "123456" }</t>
+  </si>
+  <si>
+    <t>TC_API08_008</t>
+  </si>
+  <si>
+    <t>Verify login with correct credentials</t>
+  </si>
+  <si>
+    <t>{ "email": "test1233@example.com", "password": "Abc@1234" }</t>
+  </si>
+  <si>
+    <t>{"responseCode": 200, "message": "User exists!"}</t>
+  </si>
+  <si>
+    <t>TC_API08_009</t>
+  </si>
+  <si>
+    <t>Verify login with uppercase letters in email</t>
+  </si>
+  <si>
+    <t>{ "email": "TEST1233@example.com", "password": "Abc@1234" }</t>
+  </si>
+  <si>
+    <t>TC_API08_010</t>
+  </si>
+  <si>
+    <t>Verify login with GET method instead of POST</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>Send GET request</t>
+  </si>
+  <si>
+    <t>{"responseCode": 405, "message": "This request method is not supported."}</t>
+  </si>
+  <si>
+    <t>TC_API08_011</t>
+  </si>
+  <si>
+    <t>Verify login with extra unexpected parameter</t>
+  </si>
+  <si>
+    <t>{ "email": "test1233@example.com", "password": "Abc@1234", "name": "John Smith" }</t>
+  </si>
+  <si>
+    <t>Should ignore extra
+{"responseCode": 200, "message": "User exists!"}</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>TC_API08_012</t>
+  </si>
+  <si>
+    <t>Verify login with duplicate parameters</t>
+  </si>
+  <si>
+    <t>{ "email": "test1233@example.com", "email": "test1233@example.com", "password": "Abc@1234" }</t>
+  </si>
+  <si>
     <t>TC_API11_001</t>
   </si>
   <si>
@@ -68,18 +210,12 @@
     <t>/api/createAccount</t>
   </si>
   <si>
-    <t>POST</t>
-  </si>
-  <si>
     <t>{ "name":"John Smith","email":"test1233@example.com","password":"Abc@1234","title":"Mr","birth_date":"12","birth_month":"5","birth_year":"1995","firstname":"John","lastname":"Smith","company":"TechCorp","address1":"123 Main St","address2":"Apt 4","country":"USA","zipcode":"12345","state":"California","city":"Los Angeles","mobile_number":"0123456789" }</t>
   </si>
   <si>
     <t>{"responseCode": 201, "message": "User created!"}</t>
   </si>
   <si>
-    <t>Critical</t>
-  </si>
-  <si>
     <t>TC_API11_002</t>
   </si>
   <si>
@@ -92,9 +228,6 @@
     <t>{"responseCode": 409, "message": "Email already exists!"}</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>TC_API11_003</t>
   </si>
   <si>
@@ -104,9 +237,6 @@
     <t>Omit "title", "address2", "company", "birth_date", "birth_month", and "birth_year"</t>
   </si>
   <si>
-    <t>Medium</t>
-  </si>
-  <si>
     <t>TC_API11_004</t>
   </si>
   <si>
@@ -275,9 +405,6 @@
     <t>{"responseCode": 400, "message": "Invalid birth date."}</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
     <t>TC_API11_018</t>
   </si>
   <si>
@@ -381,12 +508,6 @@
   </si>
   <si>
     <t>Verify unsupported method returns 405</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
-    <t>Send GET request</t>
   </si>
   <si>
     <r>
@@ -610,7 +731,7 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -624,9 +745,6 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -635,6 +753,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,7 +860,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A3:K4" displayName="API08_LoginWithoutEmail_Table" name="API08_LoginWithoutEmail_Table" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A3:K15" displayName="API08_LoginWithoutEmail_Table" name="API08_LoginWithoutEmail_Table" id="1">
   <tableColumns count="11">
     <tableColumn name="ID" id="1"/>
     <tableColumn name="Test Scenario" id="2"/>
@@ -758,7 +879,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A27:K54" displayName="API11_CreateAccount_Table" name="API11_CreateAccount_Table" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A18:K45" displayName="API11_CreateAccount_Table" name="API11_CreateAccount_Table" id="2">
   <tableColumns count="11">
     <tableColumn name="ID" id="1"/>
     <tableColumn name="Test Scenario" id="2"/>
@@ -777,7 +898,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A57:K72" displayName="API13_UpdateAccount_Table" name="API13_UpdateAccount_Table" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A48:K63" displayName="API13_UpdateAccount_Table" name="API13_UpdateAccount_Table" id="3">
   <tableColumns count="11">
     <tableColumn name="ID" id="1"/>
     <tableColumn name="Test Scenario" id="2"/>
@@ -1061,53 +1182,373 @@
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="G4" s="6"/>
       <c r="H4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="J4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5">
-      <c r="D5" s="1"/>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="6"/>
     </row>
     <row r="6">
-      <c r="D6" s="1"/>
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="6"/>
     </row>
     <row r="7">
-      <c r="D7" s="1"/>
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="6"/>
     </row>
     <row r="8">
-      <c r="D8" s="1"/>
+      <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="6"/>
     </row>
     <row r="9">
-      <c r="D9" s="1"/>
+      <c r="A9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="6"/>
     </row>
     <row r="10">
-      <c r="D10" s="1"/>
+      <c r="A10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="6"/>
     </row>
     <row r="11">
-      <c r="D11" s="1"/>
+      <c r="A11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="6"/>
     </row>
     <row r="12">
-      <c r="D12" s="1"/>
+      <c r="A12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="6"/>
     </row>
     <row r="13">
-      <c r="D13" s="1"/>
+      <c r="A13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="6"/>
     </row>
     <row r="14">
-      <c r="D14" s="1"/>
+      <c r="A14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="6"/>
     </row>
     <row r="15">
-      <c r="D15" s="1"/>
+      <c r="A15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="6"/>
     </row>
     <row r="16">
       <c r="D16" s="1"/>
@@ -1116,1409 +1557,1409 @@
       <c r="D17" s="1"/>
     </row>
     <row r="18">
-      <c r="D18" s="1"/>
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19">
-      <c r="D19" s="1"/>
+      <c r="A19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="9"/>
     </row>
     <row r="20">
-      <c r="D20" s="1"/>
+      <c r="A20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="9"/>
     </row>
     <row r="21">
-      <c r="D21" s="1"/>
+      <c r="A21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="9"/>
     </row>
     <row r="22">
-      <c r="D22" s="1"/>
+      <c r="A22" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="9"/>
     </row>
     <row r="23">
-      <c r="D23" s="1"/>
+      <c r="A23" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="9"/>
     </row>
     <row r="24">
-      <c r="D24" s="1"/>
+      <c r="A24" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="9"/>
     </row>
     <row r="25">
-      <c r="D25" s="1"/>
+      <c r="A25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="9"/>
     </row>
     <row r="26">
-      <c r="D26" s="1"/>
+      <c r="A26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="9"/>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A27" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="9"/>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="E28" s="4" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K28" s="9"/>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K29" s="9"/>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="G30" s="9"/>
       <c r="H30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K30" s="9"/>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>30</v>
+        <v>109</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>31</v>
+        <v>110</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>33</v>
+        <v>112</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K31" s="9"/>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>34</v>
+        <v>113</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K32" s="9"/>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>38</v>
+        <v>117</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="G33" s="9"/>
       <c r="H33" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33" s="12" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K33" s="9"/>
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="G34" s="9"/>
       <c r="H34" s="10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K34" s="9"/>
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="G35" s="9"/>
       <c r="H35" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K35" s="9"/>
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>51</v>
+        <v>130</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>52</v>
+        <v>131</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="G36" s="9"/>
       <c r="H36" s="10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K36" s="9"/>
     </row>
     <row r="37">
       <c r="A37" s="4" t="s">
-        <v>54</v>
+        <v>133</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>56</v>
+        <v>135</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="G37" s="9"/>
       <c r="H37" s="10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K37" s="9"/>
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
-        <v>58</v>
+        <v>136</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>60</v>
+        <v>138</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
       <c r="G38" s="9"/>
       <c r="H38" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K38" s="9"/>
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>17</v>
+      <c r="D39" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>64</v>
+        <v>142</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>65</v>
+        <v>143</v>
       </c>
       <c r="G39" s="9"/>
       <c r="H39" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K39" s="9"/>
     </row>
-    <row r="40">
+    <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>68</v>
+        <v>146</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>69</v>
+        <v>147</v>
       </c>
       <c r="G40" s="9"/>
       <c r="H40" s="10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K40" s="9"/>
     </row>
-    <row r="41">
+    <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>70</v>
+        <v>148</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>71</v>
+        <v>149</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>17</v>
+        <v>63</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>73</v>
+        <v>151</v>
       </c>
       <c r="G41" s="9"/>
       <c r="H41" s="10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K41" s="9"/>
     </row>
-    <row r="42">
+    <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G42" s="6"/>
+      <c r="H42" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K42" s="6"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="6"/>
+      <c r="H43" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K43" s="6"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G44" s="6"/>
+      <c r="H44" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44" s="6"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G45" s="6"/>
+      <c r="H45" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K45" s="6"/>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="A49" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G49" s="6"/>
+      <c r="H49" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K49" s="6"/>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G50" s="6"/>
+      <c r="H50" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K50" s="6"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G51" s="9"/>
+      <c r="H51" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K51" s="9"/>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E52" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="8" t="s">
+      <c r="F52" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G52" s="6"/>
+      <c r="H52" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G42" s="9"/>
-      <c r="H42" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K42" s="9"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" s="4" t="s">
+      <c r="I52" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K52" s="6"/>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" s="8" t="s">
+      <c r="F53" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G53" s="6"/>
+      <c r="H53" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G43" s="9"/>
-      <c r="H43" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I43" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K43" s="9"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="8" t="s">
+      <c r="I53" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K53" s="6"/>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="A54" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G54" s="6"/>
+      <c r="H54" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G44" s="9"/>
-      <c r="H44" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I44" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K44" s="9"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" s="8" t="s">
+      <c r="I54" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K54" s="6"/>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G55" s="6"/>
+      <c r="H55" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G45" s="9"/>
-      <c r="H45" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I45" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K45" s="9"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" s="8" t="s">
+      <c r="I55" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K55" s="6"/>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="A56" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G56" s="6"/>
+      <c r="H56" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E46" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" s="4" t="s">
+      <c r="I56" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J56" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G46" s="9"/>
-      <c r="H46" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K46" s="9"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" s="8" t="s">
+      <c r="K56" s="6"/>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="A57" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G57" s="6"/>
+      <c r="H57" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G47" s="9"/>
-      <c r="H47" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I47" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K47" s="9"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G48" s="9"/>
-      <c r="H48" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I48" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K48" s="9"/>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G49" s="9"/>
-      <c r="H49" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I49" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K49" s="9"/>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G50" s="9"/>
-      <c r="H50" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K50" s="9"/>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G51" s="6"/>
-      <c r="H51" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I51" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J51" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K51" s="6"/>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="F52" s="4" t="s">
+      <c r="I57" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J57" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G52" s="6"/>
-      <c r="H52" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I52" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="J52" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K52" s="6"/>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G53" s="6"/>
-      <c r="H53" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I53" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J53" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K53" s="6"/>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F54" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="G54" s="6"/>
-      <c r="H54" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I54" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J54" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K54" s="6"/>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="D55" s="1"/>
-    </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="D56" s="1"/>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="K57" s="6"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>126</v>
+        <v>191</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>130</v>
+        <v>167</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="G58" s="6"/>
       <c r="H58" s="7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K58" s="6"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>132</v>
+        <v>192</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>134</v>
+        <v>167</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="G59" s="6"/>
       <c r="H59" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I59" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="I59" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K59" s="6"/>
     </row>
-    <row r="60">
-      <c r="A60" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D60" s="8" t="s">
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="G60" s="6"/>
+      <c r="H60" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E60" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G60" s="9"/>
-      <c r="H60" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>29</v>
+      <c r="I60" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K60" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="K60" s="6"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>139</v>
+        <v>194</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>128</v>
+        <v>167</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>168</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="G61" s="6"/>
       <c r="H61" s="7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K61" s="6"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>142</v>
+        <v>195</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>36</v>
+        <v>167</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="G62" s="6"/>
       <c r="H62" s="7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K62" s="6"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="3" t="s">
-        <v>144</v>
+        <v>197</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>85</v>
+        <v>167</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="G63" s="6"/>
       <c r="H63" s="7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="J63" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K63" s="6"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G64" s="6"/>
-      <c r="H64" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I64" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J64" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K64" s="6"/>
+      <c r="D64" s="1"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G65" s="6"/>
-      <c r="H65" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I65" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J65" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K65" s="6"/>
+      <c r="D65" s="1"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G66" s="6"/>
-      <c r="H66" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I66" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J66" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K66" s="6"/>
+      <c r="D66" s="1"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G67" s="6"/>
-      <c r="H67" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I67" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="J67" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K67" s="6"/>
+      <c r="D67" s="1"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="G68" s="6"/>
-      <c r="H68" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I68" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="J68" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K68" s="6"/>
+      <c r="D68" s="1"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G69" s="6"/>
-      <c r="H69" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I69" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J69" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K69" s="6"/>
+      <c r="D69" s="1"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G70" s="6"/>
-      <c r="H70" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I70" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="J70" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K70" s="6"/>
+      <c r="D70" s="1"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G71" s="6"/>
-      <c r="H71" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I71" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J71" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K71" s="6"/>
+      <c r="D71" s="1"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G72" s="6"/>
-      <c r="H72" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I72" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J72" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K72" s="6"/>
+      <c r="D72" s="1"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="D73" s="1"/>
@@ -5310,39 +5751,12 @@
     <row r="1002" ht="15.75" customHeight="1">
       <c r="D1002" s="1"/>
     </row>
-    <row r="1003" ht="15.75" customHeight="1">
-      <c r="D1003" s="1"/>
-    </row>
-    <row r="1004" ht="15.75" customHeight="1">
-      <c r="D1004" s="1"/>
-    </row>
-    <row r="1005" ht="15.75" customHeight="1">
-      <c r="D1005" s="1"/>
-    </row>
-    <row r="1006" ht="15.75" customHeight="1">
-      <c r="D1006" s="1"/>
-    </row>
-    <row r="1007" ht="15.75" customHeight="1">
-      <c r="D1007" s="1"/>
-    </row>
-    <row r="1008" ht="15.75" customHeight="1">
-      <c r="D1008" s="1"/>
-    </row>
-    <row r="1009" ht="15.75" customHeight="1">
-      <c r="D1009" s="1"/>
-    </row>
-    <row r="1010" ht="15.75" customHeight="1">
-      <c r="D1010" s="1"/>
-    </row>
-    <row r="1011" ht="15.75" customHeight="1">
-      <c r="D1011" s="1"/>
-    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="I4 I28:I54 I58:I72">
+    <dataValidation type="list" allowBlank="1" sqref="I4:I15 I19:I45 I49:I63">
       <formula1>"Critical,High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H4 H28:H54 H58:H72">
+    <dataValidation type="list" allowBlank="1" sqref="H4:H15 H19:H45 H49:H63">
       <formula1>"NotTested,Pass,Fail,Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>